<commit_message>
Revert "Xiao 101 20 change"
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_CNETZEROS_CO2_province_and_sector.xlsx
+++ b/SuppXLS/Scen_CNETZEROS_CO2_province_and_sector.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="8710" firstSheet="9" activeTab="12"/>
+    <workbookView windowWidth="18340" windowHeight="8720" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="ELECO2" sheetId="21" r:id="rId1"/>
@@ -3100,7 +3100,7 @@
   <dimension ref="A1:S41"/>
   <sheetViews>
     <sheetView zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -5141,8 +5141,8 @@
   </sheetPr>
   <dimension ref="B4:L135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="H179" sqref="H179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -5225,7 +5225,7 @@
         <v>1</v>
       </c>
       <c r="L11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="4:12">
@@ -5245,7 +5245,7 @@
         <v>1</v>
       </c>
       <c r="L12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="4:12">
@@ -5265,7 +5265,7 @@
         <v>1</v>
       </c>
       <c r="L13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="4:12">
@@ -5285,7 +5285,7 @@
         <v>1</v>
       </c>
       <c r="L14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="4:12">
@@ -5305,7 +5305,7 @@
         <v>1</v>
       </c>
       <c r="L15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="4:12">
@@ -5325,7 +5325,7 @@
         <v>1</v>
       </c>
       <c r="L16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="4:12">
@@ -5345,7 +5345,7 @@
         <v>1</v>
       </c>
       <c r="L17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="4:12">
@@ -5365,7 +5365,7 @@
         <v>1</v>
       </c>
       <c r="L18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="4:12">
@@ -5385,7 +5385,7 @@
         <v>1</v>
       </c>
       <c r="L19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="4:12">
@@ -5405,7 +5405,7 @@
         <v>1</v>
       </c>
       <c r="L20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="4:12">
@@ -5425,7 +5425,7 @@
         <v>1</v>
       </c>
       <c r="L21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="4:12">
@@ -5445,7 +5445,7 @@
         <v>1</v>
       </c>
       <c r="L22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="4:12">
@@ -5465,7 +5465,7 @@
         <v>1</v>
       </c>
       <c r="L23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="4:12">
@@ -5485,7 +5485,7 @@
         <v>1</v>
       </c>
       <c r="L24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="4:12">
@@ -5505,7 +5505,7 @@
         <v>1</v>
       </c>
       <c r="L25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="4:12">
@@ -5525,7 +5525,7 @@
         <v>1</v>
       </c>
       <c r="L26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="4:12">
@@ -5545,7 +5545,7 @@
         <v>1</v>
       </c>
       <c r="L27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="4:12">
@@ -5565,7 +5565,7 @@
         <v>1</v>
       </c>
       <c r="L28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="4:12">
@@ -5585,7 +5585,7 @@
         <v>1</v>
       </c>
       <c r="L29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="4:12">
@@ -5605,7 +5605,7 @@
         <v>1</v>
       </c>
       <c r="L30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="4:12">
@@ -5625,7 +5625,7 @@
         <v>1</v>
       </c>
       <c r="L31" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="4:12">
@@ -5645,7 +5645,7 @@
         <v>1</v>
       </c>
       <c r="L32" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="4:12">
@@ -5665,7 +5665,7 @@
         <v>1</v>
       </c>
       <c r="L33" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="4:12">
@@ -5685,7 +5685,7 @@
         <v>1</v>
       </c>
       <c r="L34" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="4:12">
@@ -5705,7 +5705,7 @@
         <v>1</v>
       </c>
       <c r="L35" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="4:12">
@@ -5725,7 +5725,7 @@
         <v>1</v>
       </c>
       <c r="L36" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="4:12">
@@ -5745,7 +5745,7 @@
         <v>1</v>
       </c>
       <c r="L37" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="4:12">
@@ -5765,7 +5765,7 @@
         <v>1</v>
       </c>
       <c r="L38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="4:12">
@@ -5785,7 +5785,7 @@
         <v>1</v>
       </c>
       <c r="L39" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="4:12">
@@ -5805,7 +5805,7 @@
         <v>1</v>
       </c>
       <c r="L40" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="4:12">
@@ -5825,7 +5825,7 @@
         <v>1</v>
       </c>
       <c r="L41" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" ht="16" spans="4:12">
@@ -5844,7 +5844,7 @@
         <v>1</v>
       </c>
       <c r="L42" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="4:12">
@@ -5864,7 +5864,7 @@
         <v>1</v>
       </c>
       <c r="L43" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="4:12">
@@ -5884,7 +5884,7 @@
         <v>1</v>
       </c>
       <c r="L44" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="4:12">
@@ -5904,7 +5904,7 @@
         <v>1</v>
       </c>
       <c r="L45" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="4:12">
@@ -5924,7 +5924,7 @@
         <v>1</v>
       </c>
       <c r="L46" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="4:12">
@@ -5944,7 +5944,7 @@
         <v>1</v>
       </c>
       <c r="L47" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="4:12">
@@ -5964,7 +5964,7 @@
         <v>1</v>
       </c>
       <c r="L48" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="4:12">
@@ -5984,7 +5984,7 @@
         <v>1</v>
       </c>
       <c r="L49" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="4:12">
@@ -6004,7 +6004,7 @@
         <v>1</v>
       </c>
       <c r="L50" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="4:12">
@@ -6024,7 +6024,7 @@
         <v>1</v>
       </c>
       <c r="L51" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="4:12">
@@ -6044,7 +6044,7 @@
         <v>1</v>
       </c>
       <c r="L52" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="4:12">
@@ -6064,7 +6064,7 @@
         <v>1</v>
       </c>
       <c r="L53" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="4:12">
@@ -6084,7 +6084,7 @@
         <v>1</v>
       </c>
       <c r="L54" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="4:12">
@@ -6104,7 +6104,7 @@
         <v>1</v>
       </c>
       <c r="L55" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="4:12">
@@ -6124,7 +6124,7 @@
         <v>1</v>
       </c>
       <c r="L56" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="4:12">
@@ -6144,7 +6144,7 @@
         <v>1</v>
       </c>
       <c r="L57" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="4:12">
@@ -6164,7 +6164,7 @@
         <v>1</v>
       </c>
       <c r="L58" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="4:12">
@@ -6184,7 +6184,7 @@
         <v>1</v>
       </c>
       <c r="L59" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="4:12">
@@ -6204,7 +6204,7 @@
         <v>1</v>
       </c>
       <c r="L60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="4:12">
@@ -6224,7 +6224,7 @@
         <v>1</v>
       </c>
       <c r="L61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="4:12">
@@ -6244,7 +6244,7 @@
         <v>1</v>
       </c>
       <c r="L62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="4:12">
@@ -6264,7 +6264,7 @@
         <v>1</v>
       </c>
       <c r="L63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="4:12">
@@ -6284,7 +6284,7 @@
         <v>1</v>
       </c>
       <c r="L64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="4:12">
@@ -6304,7 +6304,7 @@
         <v>1</v>
       </c>
       <c r="L65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="4:12">
@@ -6324,7 +6324,7 @@
         <v>1</v>
       </c>
       <c r="L66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="4:12">
@@ -6344,7 +6344,7 @@
         <v>1</v>
       </c>
       <c r="L67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="4:12">
@@ -6364,7 +6364,7 @@
         <v>1</v>
       </c>
       <c r="L68" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="4:12">
@@ -6384,7 +6384,7 @@
         <v>1</v>
       </c>
       <c r="L69" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="4:12">
@@ -6404,7 +6404,7 @@
         <v>1</v>
       </c>
       <c r="L70" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="4:12">
@@ -6424,7 +6424,7 @@
         <v>1</v>
       </c>
       <c r="L71" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="4:12">
@@ -6444,7 +6444,7 @@
         <v>1</v>
       </c>
       <c r="L72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" ht="16" spans="4:12">
@@ -6463,7 +6463,7 @@
         <v>1</v>
       </c>
       <c r="L73" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="4:12">
@@ -6483,7 +6483,7 @@
         <v>1</v>
       </c>
       <c r="L74" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="4:12">
@@ -6503,7 +6503,7 @@
         <v>1</v>
       </c>
       <c r="L75" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="4:12">
@@ -6523,7 +6523,7 @@
         <v>1</v>
       </c>
       <c r="L76" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="4:12">
@@ -6543,7 +6543,7 @@
         <v>1</v>
       </c>
       <c r="L77" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="4:12">
@@ -6563,7 +6563,7 @@
         <v>1</v>
       </c>
       <c r="L78" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="4:12">
@@ -6583,7 +6583,7 @@
         <v>1</v>
       </c>
       <c r="L79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="4:12">
@@ -6603,7 +6603,7 @@
         <v>1</v>
       </c>
       <c r="L80" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="4:12">
@@ -6623,7 +6623,7 @@
         <v>1</v>
       </c>
       <c r="L81" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="4:12">
@@ -6643,7 +6643,7 @@
         <v>1</v>
       </c>
       <c r="L82" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="4:12">
@@ -6663,7 +6663,7 @@
         <v>1</v>
       </c>
       <c r="L83" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="4:12">
@@ -6683,7 +6683,7 @@
         <v>1</v>
       </c>
       <c r="L84" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="4:12">
@@ -6703,7 +6703,7 @@
         <v>1</v>
       </c>
       <c r="L85" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="4:12">
@@ -6723,7 +6723,7 @@
         <v>1</v>
       </c>
       <c r="L86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="4:12">
@@ -6743,7 +6743,7 @@
         <v>1</v>
       </c>
       <c r="L87" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="4:12">
@@ -6763,7 +6763,7 @@
         <v>1</v>
       </c>
       <c r="L88" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="4:12">
@@ -6783,7 +6783,7 @@
         <v>1</v>
       </c>
       <c r="L89" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="4:12">
@@ -6803,7 +6803,7 @@
         <v>1</v>
       </c>
       <c r="L90" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="4:12">
@@ -6823,7 +6823,7 @@
         <v>1</v>
       </c>
       <c r="L91" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="4:12">
@@ -6843,7 +6843,7 @@
         <v>1</v>
       </c>
       <c r="L92" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="4:12">
@@ -6863,7 +6863,7 @@
         <v>1</v>
       </c>
       <c r="L93" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="4:12">
@@ -6883,7 +6883,7 @@
         <v>1</v>
       </c>
       <c r="L94" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="4:12">
@@ -6903,7 +6903,7 @@
         <v>1</v>
       </c>
       <c r="L95" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="4:12">
@@ -6923,7 +6923,7 @@
         <v>1</v>
       </c>
       <c r="L96" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="4:12">
@@ -6943,7 +6943,7 @@
         <v>1</v>
       </c>
       <c r="L97" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="4:12">
@@ -6963,7 +6963,7 @@
         <v>1</v>
       </c>
       <c r="L98" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="4:12">
@@ -6983,7 +6983,7 @@
         <v>1</v>
       </c>
       <c r="L99" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="4:12">
@@ -7003,7 +7003,7 @@
         <v>1</v>
       </c>
       <c r="L100" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="4:12">
@@ -7023,7 +7023,7 @@
         <v>1</v>
       </c>
       <c r="L101" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="4:12">
@@ -7043,7 +7043,7 @@
         <v>1</v>
       </c>
       <c r="L102" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="4:12">
@@ -7063,7 +7063,7 @@
         <v>1</v>
       </c>
       <c r="L103" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" ht="16" spans="4:12">
@@ -7082,7 +7082,7 @@
         <v>1</v>
       </c>
       <c r="L104" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="4:12">
@@ -7102,7 +7102,7 @@
         <v>1</v>
       </c>
       <c r="L105" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="4:12">
@@ -7122,7 +7122,7 @@
         <v>1</v>
       </c>
       <c r="L106" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="4:12">
@@ -7142,7 +7142,7 @@
         <v>1</v>
       </c>
       <c r="L107" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="4:12">
@@ -7162,7 +7162,7 @@
         <v>1</v>
       </c>
       <c r="L108" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="4:12">
@@ -7182,7 +7182,7 @@
         <v>1</v>
       </c>
       <c r="L109" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="4:12">
@@ -7202,7 +7202,7 @@
         <v>1</v>
       </c>
       <c r="L110" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="4:12">
@@ -7222,7 +7222,7 @@
         <v>1</v>
       </c>
       <c r="L111" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="4:12">
@@ -7242,7 +7242,7 @@
         <v>1</v>
       </c>
       <c r="L112" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="4:12">
@@ -7262,7 +7262,7 @@
         <v>1</v>
       </c>
       <c r="L113" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="4:12">
@@ -7282,7 +7282,7 @@
         <v>1</v>
       </c>
       <c r="L114" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="4:12">
@@ -7302,7 +7302,7 @@
         <v>1</v>
       </c>
       <c r="L115" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="4:12">
@@ -7322,7 +7322,7 @@
         <v>1</v>
       </c>
       <c r="L116" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="4:12">
@@ -7342,7 +7342,7 @@
         <v>1</v>
       </c>
       <c r="L117" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="4:12">
@@ -7362,7 +7362,7 @@
         <v>1</v>
       </c>
       <c r="L118" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="4:12">
@@ -7382,7 +7382,7 @@
         <v>1</v>
       </c>
       <c r="L119" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="4:12">
@@ -7402,7 +7402,7 @@
         <v>1</v>
       </c>
       <c r="L120" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="4:12">
@@ -7422,7 +7422,7 @@
         <v>1</v>
       </c>
       <c r="L121" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="4:12">
@@ -7442,7 +7442,7 @@
         <v>1</v>
       </c>
       <c r="L122" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="4:12">
@@ -7462,7 +7462,7 @@
         <v>1</v>
       </c>
       <c r="L123" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="4:12">
@@ -7482,7 +7482,7 @@
         <v>1</v>
       </c>
       <c r="L124" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="4:12">
@@ -7502,7 +7502,7 @@
         <v>1</v>
       </c>
       <c r="L125" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="4:12">
@@ -7522,7 +7522,7 @@
         <v>1</v>
       </c>
       <c r="L126" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="4:12">
@@ -7542,7 +7542,7 @@
         <v>1</v>
       </c>
       <c r="L127" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="4:12">
@@ -7562,7 +7562,7 @@
         <v>1</v>
       </c>
       <c r="L128" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="4:12">
@@ -7582,7 +7582,7 @@
         <v>1</v>
       </c>
       <c r="L129" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="4:12">
@@ -7602,7 +7602,7 @@
         <v>1</v>
       </c>
       <c r="L130" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="4:12">
@@ -7622,7 +7622,7 @@
         <v>1</v>
       </c>
       <c r="L131" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="4:12">
@@ -7642,7 +7642,7 @@
         <v>1</v>
       </c>
       <c r="L132" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="4:12">
@@ -7662,7 +7662,7 @@
         <v>1</v>
       </c>
       <c r="L133" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="4:12">
@@ -7682,7 +7682,7 @@
         <v>1</v>
       </c>
       <c r="L134" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135" ht="16" spans="7:7">
@@ -7701,8 +7701,8 @@
   </sheetPr>
   <dimension ref="B4:L164"/>
   <sheetViews>
-    <sheetView zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -16337,7 +16337,7 @@
   <sheetPr/>
   <dimension ref="B4:N41"/>
   <sheetViews>
-    <sheetView zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>

</xml_diff>